<commit_message>
prop, dest ctr, cvtr failed
</commit_message>
<xml_diff>
--- a/model_log.xlsx
+++ b/model_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
   <si>
     <t>0.529; 0.498; 0.497</t>
   </si>
@@ -173,6 +173,13 @@
   <si>
     <t>0503_lgbmranker_v2</t>
   </si>
+  <si>
+    <t>0503_lgbmranker_v2_sparse_features</t>
+  </si>
+  <si>
+    <t>1. negative value in sparse features
+2. null value not fixed</t>
+  </si>
 </sst>
 </file>
 
@@ -180,8 +187,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -209,6 +216,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -217,8 +232,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,96 +316,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -330,9 +324,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,6 +333,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,181 +379,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,11 +662,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,7 +681,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,6 +697,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,172 +744,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -950,6 +957,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1270,15 +1280,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="C2:Q34"/>
+  <dimension ref="C2:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="21.609375" customWidth="1"/>
+    <col min="3" max="3" width="30.984375" customWidth="1"/>
     <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="16" max="17" width="12.6875"/>
   </cols>
@@ -1469,16 +1479,30 @@
         <v>0.966101694915254</v>
       </c>
     </row>
-    <row r="10" spans="5:15">
+    <row r="10" ht="112" spans="3:18">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="H10" s="7"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
+      <c r="J10" s="6">
+        <v>147</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.687</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.494</v>
+      </c>
+      <c r="M10" s="15">
+        <v>0.5</v>
+      </c>
       <c r="N10" s="14"/>
       <c r="O10" s="19"/>
+      <c r="R10" s="21" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="5:15">
       <c r="E11" s="6"/>

</xml_diff>